<commit_message>
updated results and intermediate files
</commit_message>
<xml_diff>
--- a/results/tables/models_pd.xlsx
+++ b/results/tables/models_pd.xlsx
@@ -414,16 +414,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.2722086851428571</v>
+        <v>-0.2870643238427826</v>
       </c>
       <c r="C2">
-        <v>-1.234393124515712</v>
+        <v>-1.213958938283074</v>
       </c>
       <c r="D2">
-        <v>0.5558395939339619</v>
+        <v>0.6571227527281447</v>
       </c>
       <c r="E2">
-        <v>0.4880034275921166</v>
+        <v>0.4841473864610111</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -431,13 +431,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>0.01522572123317697</v>
+        <v>0.01518785678901663</v>
       </c>
       <c r="H2">
-        <v>2.062137752364779E-08</v>
+        <v>4.336090312679973E-10</v>
       </c>
       <c r="I2">
-        <v>0.1031068228910795</v>
+        <v>0.1114465384825023</v>
       </c>
     </row>
     <row r="3">
@@ -447,16 +447,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.053703767048436</v>
+        <v>0.06246785514814768</v>
       </c>
       <c r="C3">
-        <v>-0.3371887809868777</v>
+        <v>-0.3240844722207426</v>
       </c>
       <c r="D3">
-        <v>0.4763425689503425</v>
+        <v>0.5243877783215349</v>
       </c>
       <c r="E3">
-        <v>0.7759211653813196</v>
+        <v>0.7527849185946873</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -464,13 +464,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>0.3200245453080248</v>
+        <v>0.3181110463215805</v>
       </c>
       <c r="H3">
-        <v>0.0407042360185913</v>
+        <v>0.03795643452122212</v>
       </c>
       <c r="I3">
-        <v>0.5524459814987401</v>
+        <v>0.5479150678513206</v>
       </c>
     </row>
     <row r="4">
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.612488716373465</v>
+        <v>0.6060071755630394</v>
       </c>
       <c r="C4">
-        <v>0.003026170857226709</v>
+        <v>0.004055495560704211</v>
       </c>
       <c r="D4">
-        <v>1.199093884763059</v>
+        <v>1.192054586825716</v>
       </c>
     </row>
     <row r="5">
@@ -496,13 +496,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.5124949152685262</v>
+        <v>0.5186528085313554</v>
       </c>
       <c r="C5">
-        <v>2.011084829627446E-05</v>
+        <v>5.60036937795076E-06</v>
       </c>
       <c r="D5">
-        <v>1.49983600149125</v>
+        <v>1.49585596558568</v>
       </c>
     </row>
   </sheetData>
@@ -572,16 +572,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-2.055200952853435</v>
+        <v>-2.069507545374689</v>
       </c>
       <c r="C2">
-        <v>-3.33250253151034</v>
+        <v>-3.295465335415409</v>
       </c>
       <c r="D2">
-        <v>-0.879342675090479</v>
+        <v>-0.8359086681387676</v>
       </c>
       <c r="E2">
-        <v>0.005141388174807249</v>
+        <v>0.006855184233076184</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -589,13 +589,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>0.01944254071019452</v>
+        <v>0.01507050511751816</v>
       </c>
       <c r="H2">
-        <v>2.133755873510566E-10</v>
+        <v>2.650000550675009E-10</v>
       </c>
       <c r="I2">
-        <v>0.1304189574927263</v>
+        <v>0.1132267775161799</v>
       </c>
     </row>
     <row r="3">
@@ -605,16 +605,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.14397800005794</v>
+        <v>-0.1094296970220441</v>
       </c>
       <c r="C3">
-        <v>-0.6080655455973637</v>
+        <v>-0.5919154831931398</v>
       </c>
       <c r="D3">
-        <v>0.3267044062354572</v>
+        <v>0.346977032977319</v>
       </c>
       <c r="E3">
-        <v>0.5325621251071122</v>
+        <v>0.6251071122536418</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>0.3375157852339059</v>
+        <v>0.3523991642135738</v>
       </c>
       <c r="H3">
-        <v>0.05886900139060895</v>
+        <v>0.08454266992975468</v>
       </c>
       <c r="I3">
-        <v>0.5440526604377653</v>
+        <v>0.5651828635195373</v>
       </c>
     </row>
     <row r="4">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.5305321357419133</v>
+        <v>0.5468644997283544</v>
       </c>
       <c r="C4">
-        <v>0.0007248036040148385</v>
+        <v>0.0006550715212962707</v>
       </c>
       <c r="D4">
-        <v>1.157560919482638</v>
+        <v>1.151798602178438</v>
       </c>
     </row>
     <row r="5">
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.8879388185845519</v>
+        <v>0.907150703699853</v>
       </c>
       <c r="C5">
-        <v>0.0001308016855700164</v>
+        <v>0.0001736751018040655</v>
       </c>
       <c r="D5">
-        <v>2.242888989805669</v>
+        <v>2.229846172697675</v>
       </c>
     </row>
   </sheetData>
@@ -730,16 +730,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.9473666591154387</v>
+        <v>-0.9275644248602527</v>
       </c>
       <c r="C2">
-        <v>-1.986689322973193</v>
+        <v>-2.021174175828682</v>
       </c>
       <c r="D2">
-        <v>0.1720023958619913</v>
+        <v>0.1781684828495378</v>
       </c>
       <c r="E2">
-        <v>0.06940874035989708</v>
+        <v>0.07497857754927173</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -747,13 +747,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>0.01062789580348386</v>
+        <v>0.0112702969106404</v>
       </c>
       <c r="H2">
-        <v>7.324507358356352E-10</v>
+        <v>1.168747347216687E-10</v>
       </c>
       <c r="I2">
-        <v>0.08406312247172157</v>
+        <v>0.09208769738712898</v>
       </c>
     </row>
     <row r="3">
@@ -763,16 +763,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.01508047116019801</v>
+        <v>0.01281899394636703</v>
       </c>
       <c r="C3">
-        <v>-0.3005688709806447</v>
+        <v>-0.3222326932963732</v>
       </c>
       <c r="D3">
-        <v>0.3161791395371858</v>
+        <v>0.3310391849863202</v>
       </c>
       <c r="E3">
-        <v>0.914738646101114</v>
+        <v>0.9284490145672666</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -780,13 +780,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>0.4240865369919747</v>
+        <v>0.3977535799041945</v>
       </c>
       <c r="H3">
-        <v>0.1459895666467537</v>
+        <v>0.1175956927889487</v>
       </c>
       <c r="I3">
-        <v>0.6364258954169015</v>
+        <v>0.6104745505746456</v>
       </c>
     </row>
     <row r="4">
@@ -796,13 +796,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.4088585195415334</v>
+        <v>0.3772554572548459</v>
       </c>
       <c r="C4">
-        <v>0.0007096209185546481</v>
+        <v>6.384747985893152E-05</v>
       </c>
       <c r="D4">
-        <v>0.902226145445568</v>
+        <v>0.8610929354152685</v>
       </c>
     </row>
     <row r="5">
@@ -812,13 +812,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.8189120740801519</v>
+        <v>0.8183031899752338</v>
       </c>
       <c r="C5">
-        <v>0.003580748142496253</v>
+        <v>0.001003705964852943</v>
       </c>
       <c r="D5">
-        <v>2.008831922986223</v>
+        <v>1.99096592208239</v>
       </c>
     </row>
   </sheetData>
@@ -888,16 +888,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-6.048829973982603</v>
+        <v>-6.116724577228305</v>
       </c>
       <c r="C2">
-        <v>-7.505848684459273</v>
+        <v>-7.574624260268472</v>
       </c>
       <c r="D2">
-        <v>-4.534543153719069</v>
+        <v>-4.571076654326432</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0004284490145671782</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -905,13 +905,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>0.09984940079129859</v>
+        <v>0.08847559383205764</v>
       </c>
       <c r="H2">
-        <v>8.342339011363359E-11</v>
+        <v>1.31696401501414E-07</v>
       </c>
       <c r="I2">
-        <v>0.2759633251975892</v>
+        <v>0.2676651759927107</v>
       </c>
     </row>
     <row r="3">
@@ -921,16 +921,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.663318052694679</v>
+        <v>-0.6386565865471112</v>
       </c>
       <c r="C3">
-        <v>-1.392285442725598</v>
+        <v>-1.497441672046309</v>
       </c>
       <c r="D3">
-        <v>0.08553947778223453</v>
+        <v>0.1164906822615449</v>
       </c>
       <c r="E3">
-        <v>0.08740359897172234</v>
+        <v>0.1135389888603255</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -938,13 +938,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>0.2927614822437667</v>
+        <v>0.2657690043821767</v>
       </c>
       <c r="H3">
-        <v>0.04163407119617186</v>
+        <v>0.03286038096274363</v>
       </c>
       <c r="I3">
-        <v>0.5153664827007203</v>
+        <v>0.4929916174201059</v>
       </c>
     </row>
     <row r="4">
@@ -954,13 +954,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.7738948825396216</v>
+        <v>0.7532221810628891</v>
       </c>
       <c r="C4">
-        <v>0.0004419868057175594</v>
+        <v>0.0006079170835843788</v>
       </c>
       <c r="D4">
-        <v>1.722280937788695</v>
+        <v>1.697642035587546</v>
       </c>
     </row>
     <row r="5">
@@ -970,13 +970,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.8603055063156431</v>
+        <v>0.857282876066121</v>
       </c>
       <c r="C5">
-        <v>0.0003361497742627412</v>
+        <v>0.000437916461978934</v>
       </c>
       <c r="D5">
-        <v>2.296931864146965</v>
+        <v>2.324973984042936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>